<commit_message>
SSDM-13256: Removed "Auto generate code" and "$" from the list of attributes.
</commit_message>
<xml_diff>
--- a/server-application-server/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-sample-filtered-fields.xlsx
+++ b/server-application-server/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-sample-filtered-fields.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
   <si>
     <t xml:space="preserve">SAMPLE</t>
   </si>
@@ -31,9 +31,6 @@
     <t xml:space="preserve">DEFAULT</t>
   </si>
   <si>
-    <t xml:space="preserve">$</t>
-  </si>
-  <si>
     <t xml:space="preserve">Identifier</t>
   </si>
   <si>
@@ -49,16 +46,10 @@
     <t xml:space="preserve">Experiment</t>
   </si>
   <si>
-    <t xml:space="preserve">Auto generate code</t>
-  </si>
-  <si>
     <t xml:space="preserve">/DEFAULT/DEFAULT/DEFAULT</t>
   </si>
   <si>
     <t xml:space="preserve">/DEFAULT/DEFAULT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FALSE</t>
   </si>
   <si>
     <t xml:space="preserve">STORAGE</t>
@@ -109,9 +100,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
   <fonts count="10">
     <font>
@@ -226,7 +216,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -265,10 +255,6 @@
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -300,7 +286,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ14"/>
+  <dimension ref="A1:XFD14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
@@ -313,10 +299,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="13.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="24.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="31.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="23.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="33.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1023" style="1" width="8.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="23.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="33.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="1022" style="1" width="8.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="1" width="8.37"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -324,7 +310,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3"/>
-      <c r="H1" s="3"/>
+      <c r="G1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
@@ -342,13 +328,13 @@
       <c r="E3" s="6"/>
     </row>
     <row r="4" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -357,39 +343,34 @@
       <c r="E4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="AMG4" s="1"/>
+      <c r="XFD4" s="0"/>
+    </row>
+    <row r="5" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9"/>
-    </row>
-    <row r="5" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="3" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" s="11"/>
-      <c r="I5" s="12"/>
+        <v>8</v>
+      </c>
+      <c r="F5" s="10"/>
+      <c r="G5" s="11"/>
+      <c r="AMG5" s="1"/>
+      <c r="XFD5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="7" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -397,7 +378,7 @@
         <v>0</v>
       </c>
       <c r="B7" s="3"/>
-      <c r="H7" s="3"/>
+      <c r="G7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
@@ -410,121 +391,96 @@
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E9" s="6"/>
     </row>
     <row r="10" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" s="0"/>
+        <v>13</v>
+      </c>
+      <c r="F10" s="9"/>
       <c r="G10" s="9"/>
       <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
+      <c r="AMD10" s="1"/>
       <c r="AME10" s="1"/>
-      <c r="AMF10" s="1"/>
-      <c r="AMI10" s="0"/>
-      <c r="AMJ10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="11" t="n">
+        <v>15</v>
+      </c>
+      <c r="C11" s="10" t="n">
         <v>9999</v>
       </c>
-      <c r="D11" s="11"/>
-      <c r="E11" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="F11" s="0"/>
-      <c r="G11" s="0"/>
-      <c r="H11" s="0"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="AMD11" s="1"/>
       <c r="AME11" s="1"/>
-      <c r="AMF11" s="1"/>
-      <c r="AMI11" s="0"/>
-      <c r="AMJ11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="11" t="n">
+        <v>18</v>
+      </c>
+      <c r="C12" s="10" t="n">
         <v>1111</v>
       </c>
-      <c r="E12" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="F12" s="0"/>
-      <c r="G12" s="0"/>
-      <c r="H12" s="0"/>
+      <c r="E12" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="AMD12" s="1"/>
       <c r="AME12" s="1"/>
-      <c r="AMF12" s="1"/>
-      <c r="AMI12" s="0"/>
-      <c r="AMJ12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="129.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C13" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D13" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="E13" s="0"/>
-      <c r="F13" s="0"/>
-      <c r="G13" s="0"/>
-      <c r="H13" s="0"/>
+      <c r="D13" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="AMD13" s="1"/>
       <c r="AME13" s="1"/>
-      <c r="AMF13" s="1"/>
-      <c r="AMI13" s="0"/>
-      <c r="AMJ13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="129.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C14" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D14" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="E14" s="0"/>
-      <c r="F14" s="0"/>
-      <c r="G14" s="0"/>
-      <c r="H14" s="0"/>
+      <c r="D14" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="AMD14" s="1"/>
       <c r="AME14" s="1"/>
-      <c r="AMF14" s="1"/>
-      <c r="AMI14" s="0"/>
-      <c r="AMJ14" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>